<commit_message>
last commit before deleting .idea
</commit_message>
<xml_diff>
--- a/static/excels/Habitat.xlsx
+++ b/static/excels/Habitat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idaca\DjangoProjects\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idaca\DjangoProjects\wtp\static\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECC4276-CF65-4514-8D7C-9B546D10E7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8822E2EC-B220-4693-9109-71DD9F674A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2460" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Habitat" sheetId="1" r:id="rId1"/>
@@ -427,14 +427,14 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -442,254 +442,254 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
+      <c r="E2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
+      <c r="E3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
+      <c r="E5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
+      <c r="E6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
+      <c r="E7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10">
-        <v>4</v>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
+      <c r="E13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
+      <c r="E14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15">
-        <v>4</v>
+      <c r="E15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>